<commit_message>
feat: final version for reuse component
</commit_message>
<xml_diff>
--- a/packages/orders/files/User_1row_complete.xlsx
+++ b/packages/orders/files/User_1row_complete.xlsx
@@ -5,18 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\hacking-away-sampleapp\packages\orders\webapp\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UI5\hacking-away-sampleapp\packages\orders\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34351C14-8ADE-4D2C-8DF2-F0B97958095C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366A105-9F89-456C-8164-E039A7AADC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -415,7 +414,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>